<commit_message>
* Indicator command * Mapping command revisited to allow specifying many-to-many mappings * A new function in helper, "augment_dataframe_with_mapped_columns" to support ETL considering many-to-many mappngs (this last still not done) * Refactoring of import and export modules: from "external_sources" to "ie_imports" and "exports" to "ie_exports" * Empty modules just considering possible export formats: BI cubes, graphs, LCA, RDF, SDMX * Refactoring of package to make explicit where MAGIC project specific integrations will be placed
</commit_message>
<xml_diff>
--- a/backend_tests/z_input_files/test_spreadsheet_2.xlsx
+++ b/backend_tests/z_input_files/test_spreadsheet_2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="110">
   <si>
     <t xml:space="preserve">Case study code</t>
   </si>
@@ -298,6 +298,18 @@
   </si>
   <si>
     <t xml:space="preserve">MCR2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Child</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scaled factor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source</t>
   </si>
   <si>
     <t xml:space="preserve">Typologies of farms defined by patterns of crops </t>
@@ -768,7 +780,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.37"/>
   </cols>
@@ -918,14 +930,14 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="8.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="32.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="38.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="38.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="8.37"/>
   </cols>
   <sheetData>
@@ -2085,7 +2097,7 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="8.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.16"/>
@@ -2347,10 +2359,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:E15"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2359,156 +2371,144 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.37"/>
   </cols>
   <sheetData>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="7" t="s">
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C3" s="8" t="s">
+      <c r="B1" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-    </row>
+      <c r="C1" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="9"/>
-      <c r="C4" s="10" t="s">
+      <c r="B4" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C5" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="9"/>
+      <c r="C6" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10" t="s">
+      <c r="D6" s="10"/>
+      <c r="E6" s="10" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="C5" s="10" t="s">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D7" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E7" s="10" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="11" t="s">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="12" t="n">
+      <c r="C8" s="12" t="n">
         <v>0.151660472365424</v>
       </c>
-      <c r="D6" s="13" t="n">
+      <c r="D8" s="13" t="n">
         <v>0.119641076769691</v>
       </c>
-      <c r="E6" s="14" t="n">
+      <c r="E8" s="14" t="n">
         <v>0</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="C7" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" s="16" t="n">
-        <v>0.191674975074776</v>
-      </c>
-      <c r="E7" s="17" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="C8" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="D8" s="16" t="n">
-        <v>0.0249252243270189</v>
-      </c>
-      <c r="E8" s="17" t="n">
-        <v>0.02</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="15" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="C9" s="15" t="n">
         <v>0</v>
       </c>
       <c r="D9" s="16" t="n">
-        <v>0.038218677301429</v>
+        <v>0.191674975074776</v>
       </c>
       <c r="E9" s="17" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="C10" s="18" t="n">
-        <v>0.4203332933701</v>
+        <v>98</v>
+      </c>
+      <c r="C10" s="15" t="n">
+        <v>0</v>
       </c>
       <c r="D10" s="16" t="n">
-        <v>0.206048521103357</v>
+        <v>0.0249252243270189</v>
       </c>
       <c r="E10" s="17" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="C11" s="18" t="n">
-        <v>0.428006234264477</v>
+        <v>99</v>
+      </c>
+      <c r="C11" s="15" t="n">
+        <v>0</v>
       </c>
       <c r="D11" s="16" t="n">
-        <v>0.291625124626122</v>
+        <v>0.038218677301429</v>
       </c>
       <c r="E11" s="17" t="n">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="C12" s="15" t="n">
-        <v>0</v>
+        <v>100</v>
+      </c>
+      <c r="C12" s="18" t="n">
+        <v>0.4203332933701</v>
       </c>
       <c r="D12" s="16" t="n">
-        <v>0.0510136257892988</v>
+        <v>0.206048521103357</v>
       </c>
       <c r="E12" s="17" t="n">
-        <v>0.14</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="C13" s="15" t="n">
-        <v>0</v>
+        <v>101</v>
+      </c>
+      <c r="C13" s="18" t="n">
+        <v>0.428006234264477</v>
       </c>
       <c r="D13" s="16" t="n">
-        <v>0.0768527750083084</v>
+        <v>0.291625124626122</v>
       </c>
       <c r="E13" s="17" t="n">
         <v>0.01</v>
@@ -2516,37 +2516,65 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="15" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C14" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="D14" s="0" t="n">
+      <c r="D14" s="16" t="n">
+        <v>0.0510136257892988</v>
+      </c>
+      <c r="E14" s="17" t="n">
+        <v>0.14</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="C15" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="E14" s="17" t="n">
+      <c r="D15" s="16" t="n">
+        <v>0.0768527750083084</v>
+      </c>
+      <c r="E15" s="17" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="C16" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" s="17" t="n">
         <v>0.68</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="19" t="s">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="C15" s="19" t="n">
+      <c r="C17" s="19" t="n">
         <v>0</v>
       </c>
-      <c r="D15" s="20" t="n">
+      <c r="D17" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="E15" s="21" t="n">
+      <c r="E17" s="21" t="n">
         <v>0.04</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2578,7 +2606,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>29</v>
@@ -2613,13 +2641,13 @@
         <v>47</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>213</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2680,7 +2708,7 @@
   </sheetPr>
   <dimension ref="B3:E12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -2693,7 +2721,7 @@
   <sheetData>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="7" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
@@ -2702,7 +2730,7 @@
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="22"/>
       <c r="C4" s="8" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
@@ -2719,7 +2747,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="10" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>84</v>

</xml_diff>

<commit_message>
* Upscale command, first approach, completed. Tested using test file "test_spreadsheet_2.xlsx", a shortened version of Almeria case study. * Other features have just been sketched
</commit_message>
<xml_diff>
--- a/backend_tests/z_input_files/test_spreadsheet_2.xlsx
+++ b/backend_tests/z_input_files/test_spreadsheet_2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="102">
   <si>
     <t xml:space="preserve">Case study code</t>
   </si>
@@ -300,58 +300,34 @@
     <t xml:space="preserve">MCR2</t>
   </si>
   <si>
-    <t xml:space="preserve">Parent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Child</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scaled factor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Source</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Typologies of farms defined by patterns of crops </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Land use pattern (%)</t>
+    <t xml:space="preserve">LU</t>
   </si>
   <si>
     <t xml:space="preserve">Crop / Farm</t>
   </si>
   <si>
-    <t xml:space="preserve">Green bean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Melon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pepper</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tomato</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Watermelon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zuchini</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lettuce</t>
-  </si>
-  <si>
     <t xml:space="preserve">AgrarianRegionID</t>
   </si>
   <si>
-    <t xml:space="preserve">LU</t>
+    <t xml:space="preserve">AR1</t>
   </si>
   <si>
     <t xml:space="preserve">ha</t>
   </si>
   <si>
-    <t xml:space="preserve">Typologies of agrarian regions defined by patterns of farms</t>
+    <t xml:space="preserve">AR2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AR3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AR4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AR5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AR6</t>
   </si>
   <si>
     <t xml:space="preserve">Farm / AgrarianRegion</t>
@@ -361,12 +337,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0"/>
     <numFmt numFmtId="166" formatCode="0.00%"/>
     <numFmt numFmtId="167" formatCode="0.00"/>
-    <numFmt numFmtId="168" formatCode="0.0"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -429,7 +404,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -438,24 +413,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFBF9000"/>
-        <bgColor rgb="FF808000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFD966"/>
-        <bgColor rgb="FFFFFF99"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFE7E6E6"/>
         <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -467,13 +430,6 @@
       <left style="thin"/>
       <right style="thin"/>
       <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top/>
       <bottom style="thin"/>
       <diagonal/>
     </border>
@@ -595,23 +551,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -619,54 +579,54 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -675,23 +635,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -745,12 +701,12 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFD966"/>
+      <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFBF9000"/>
+      <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
@@ -780,7 +736,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.37"/>
   </cols>
@@ -937,7 +893,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="32.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="38.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="38.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="8.37"/>
   </cols>
   <sheetData>
@@ -2359,55 +2315,46 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.37"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>94</v>
-      </c>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="7" t="s">
-        <v>95</v>
-      </c>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="7"/>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="8"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="9"/>
+      <c r="B6" s="9" t="s">
+        <v>91</v>
+      </c>
       <c r="C6" s="10" t="s">
         <v>38</v>
       </c>
@@ -2416,9 +2363,9 @@
         <v>70</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="9" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>84</v>
@@ -2460,7 +2407,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="15" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
       <c r="C10" s="15" t="n">
         <v>0</v>
@@ -2473,107 +2420,30 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="C11" s="15" t="n">
+      <c r="B11" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="C11" s="18" t="n">
         <v>0</v>
       </c>
-      <c r="D11" s="16" t="n">
-        <v>0.038218677301429</v>
-      </c>
-      <c r="E11" s="17" t="n">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="C12" s="18" t="n">
-        <v>0.4203332933701</v>
-      </c>
-      <c r="D12" s="16" t="n">
-        <v>0.206048521103357</v>
-      </c>
-      <c r="E12" s="17" t="n">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="C13" s="18" t="n">
-        <v>0.428006234264477</v>
-      </c>
-      <c r="D13" s="16" t="n">
-        <v>0.291625124626122</v>
-      </c>
-      <c r="E13" s="17" t="n">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="C14" s="15" t="n">
+      <c r="D11" s="19" t="n">
         <v>0</v>
       </c>
-      <c r="D14" s="16" t="n">
-        <v>0.0510136257892988</v>
-      </c>
-      <c r="E14" s="17" t="n">
-        <v>0.14</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="C15" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="D15" s="16" t="n">
-        <v>0.0768527750083084</v>
-      </c>
-      <c r="E15" s="17" t="n">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="C16" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="D16" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E16" s="17" t="n">
-        <v>0.68</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="C17" s="19" t="n">
-        <v>0</v>
-      </c>
-      <c r="D17" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="E17" s="21" t="n">
+      <c r="E11" s="20" t="n">
         <v>0.04</v>
       </c>
     </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="C5:E5"/>
+  <mergeCells count="1">
     <mergeCell ref="C6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2593,8 +2463,8 @@
   </sheetPr>
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2606,7 +2476,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>29</v>
@@ -2633,61 +2503,106 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>1</v>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>94</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>47</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>213</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>2</v>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>91</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>28609</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>3</v>
+      <c r="E3" s="0" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>91</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>12073</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <v>4</v>
+      <c r="E4" s="0" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>91</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>10160</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
-        <v>5</v>
+      <c r="E5" s="0" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>91</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>341</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
-        <v>6</v>
+      <c r="E6" s="0" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>91</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>384</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -2709,34 +2624,32 @@
   <dimension ref="B3:E12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.37"/>
   </cols>
   <sheetData>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="7" t="s">
-        <v>108</v>
-      </c>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="7"/>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="22"/>
-      <c r="C4" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="22"/>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="21"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="22" t="s">
+        <v>91</v>
+      </c>
       <c r="C5" s="10" t="s">
         <v>38</v>
       </c>
@@ -2747,7 +2660,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="10" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>84</v>
@@ -2760,8 +2673,8 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="24" t="n">
-        <v>1</v>
+      <c r="B7" s="24" t="s">
+        <v>94</v>
       </c>
       <c r="C7" s="12" t="n">
         <v>0</v>
@@ -2774,8 +2687,8 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="24" t="n">
-        <v>2</v>
+      <c r="B8" s="24" t="s">
+        <v>96</v>
       </c>
       <c r="C8" s="26" t="n">
         <v>0.15</v>
@@ -2788,8 +2701,8 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="24" t="n">
-        <v>3</v>
+      <c r="B9" s="24" t="s">
+        <v>97</v>
       </c>
       <c r="C9" s="26" t="n">
         <v>0.19</v>
@@ -2802,8 +2715,8 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="24" t="n">
-        <v>4</v>
+      <c r="B10" s="24" t="s">
+        <v>98</v>
       </c>
       <c r="C10" s="26" t="n">
         <v>0.03</v>
@@ -2816,8 +2729,8 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="24" t="n">
-        <v>5</v>
+      <c r="B11" s="24" t="s">
+        <v>99</v>
       </c>
       <c r="C11" s="26" t="n">
         <v>0</v>
@@ -2830,8 +2743,8 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="28" t="n">
-        <v>6</v>
+      <c r="B12" s="28" t="s">
+        <v>100</v>
       </c>
       <c r="C12" s="29" t="n">
         <v>0</v>
@@ -2844,9 +2757,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="C4:E4"/>
+  <mergeCells count="1">
     <mergeCell ref="C5:D5"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>